<commit_message>
Updated data from R23
</commit_message>
<xml_diff>
--- a/data/f1_fantasy_archive.xlsx
+++ b/data/f1_fantasy_archive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexs\Dropbox\Dev\f1_fantasy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32398731-C7BF-450C-89EE-32855A5D4089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77149FA0-1509-474A-89AC-C5A0FAC330E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="8" xr2:uid="{5075C4C2-DC0E-48A5-BDF1-482703F248E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="8" xr2:uid="{5075C4C2-DC0E-48A5-BDF1-482703F248E6}"/>
   </bookViews>
   <sheets>
     <sheet name="2023 Drivers Points" sheetId="1" r:id="rId1"/>
@@ -2197,815 +2197,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2707B16-05A3-42D1-BE37-AF149E8BEDBE}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V12" sqref="V12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="3">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3">
-        <v>16</v>
-      </c>
-      <c r="R1" s="3">
-        <v>17</v>
-      </c>
-      <c r="S1" s="3">
-        <v>18</v>
-      </c>
-      <c r="T1" s="3">
-        <v>19</v>
-      </c>
-      <c r="U1" s="3">
-        <v>20</v>
-      </c>
-      <c r="V1" s="3">
-        <v>21</v>
-      </c>
-      <c r="W1" s="3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2">
-        <v>71</v>
-      </c>
-      <c r="C2" s="2">
-        <v>101</v>
-      </c>
-      <c r="D2" s="2">
-        <v>71</v>
-      </c>
-      <c r="E2" s="2">
-        <v>92</v>
-      </c>
-      <c r="F2" s="2">
-        <v>86</v>
-      </c>
-      <c r="G2" s="2">
-        <v>118</v>
-      </c>
-      <c r="H2" s="2">
-        <v>82</v>
-      </c>
-      <c r="I2" s="2">
-        <v>83</v>
-      </c>
-      <c r="J2" s="2">
-        <v>88</v>
-      </c>
-      <c r="K2" s="2">
-        <v>40</v>
-      </c>
-      <c r="L2" s="2">
-        <v>100</v>
-      </c>
-      <c r="M2" s="2">
-        <v>90</v>
-      </c>
-      <c r="N2" s="2">
-        <v>93</v>
-      </c>
-      <c r="O2" s="2">
-        <v>100</v>
-      </c>
-      <c r="P2" s="2">
-        <v>52</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>97</v>
-      </c>
-      <c r="R2" s="2">
-        <v>6</v>
-      </c>
-      <c r="S2" s="2">
-        <v>64</v>
-      </c>
-      <c r="T2" s="2">
-        <v>22</v>
-      </c>
-      <c r="U2" s="2">
-        <v>86</v>
-      </c>
-      <c r="V2" s="2">
-        <v>63</v>
-      </c>
-      <c r="W2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23">
-      <c r="A3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2">
-        <v>36</v>
-      </c>
-      <c r="C3" s="2">
-        <v>-23</v>
-      </c>
-      <c r="D3" s="2">
-        <v>56</v>
-      </c>
-      <c r="E3" s="2">
-        <v>73</v>
-      </c>
-      <c r="F3" s="2">
-        <v>64</v>
-      </c>
-      <c r="G3" s="2">
-        <v>34</v>
-      </c>
-      <c r="H3" s="2">
-        <v>67</v>
-      </c>
-      <c r="I3" s="2">
-        <v>71</v>
-      </c>
-      <c r="J3" s="2">
-        <v>61</v>
-      </c>
-      <c r="K3" s="2">
-        <v>57</v>
-      </c>
-      <c r="L3" s="2">
-        <v>67</v>
-      </c>
-      <c r="M3" s="2">
-        <v>41</v>
-      </c>
-      <c r="N3" s="2">
-        <v>70</v>
-      </c>
-      <c r="O3" s="2">
-        <v>39</v>
-      </c>
-      <c r="P3" s="2">
-        <v>-4</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>67</v>
-      </c>
-      <c r="R3" s="2">
-        <v>28</v>
-      </c>
-      <c r="S3" s="2">
-        <v>48</v>
-      </c>
-      <c r="T3" s="2">
-        <v>85</v>
-      </c>
-      <c r="U3" s="2">
-        <v>58</v>
-      </c>
-      <c r="V3" s="2">
-        <v>-2</v>
-      </c>
-      <c r="W3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="2">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2">
-        <v>67</v>
-      </c>
-      <c r="D4" s="2">
-        <v>46</v>
-      </c>
-      <c r="E4" s="2">
-        <v>46</v>
-      </c>
-      <c r="F4" s="2">
-        <v>21</v>
-      </c>
-      <c r="G4" s="2">
-        <v>60</v>
-      </c>
-      <c r="H4" s="2">
-        <v>71</v>
-      </c>
-      <c r="I4" s="2">
-        <v>23</v>
-      </c>
-      <c r="J4" s="2">
-        <v>28</v>
-      </c>
-      <c r="K4" s="2">
-        <v>51</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2">
-        <v>41</v>
-      </c>
-      <c r="N4" s="2">
-        <v>55</v>
-      </c>
-      <c r="O4" s="2">
-        <v>39</v>
-      </c>
-      <c r="P4" s="2">
-        <v>47</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>56</v>
-      </c>
-      <c r="R4" s="2">
-        <v>85</v>
-      </c>
-      <c r="S4" s="2">
-        <v>51</v>
-      </c>
-      <c r="T4" s="2">
-        <v>92</v>
-      </c>
-      <c r="U4" s="2">
-        <v>36</v>
-      </c>
-      <c r="V4" s="2">
-        <v>95</v>
-      </c>
-      <c r="W4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23">
-      <c r="A5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="2">
-        <v>67</v>
-      </c>
-      <c r="C5" s="2">
-        <v>69</v>
-      </c>
-      <c r="D5" s="2">
-        <v>56</v>
-      </c>
-      <c r="E5" s="2">
-        <v>60</v>
-      </c>
-      <c r="F5" s="2">
-        <v>46</v>
-      </c>
-      <c r="G5" s="2">
-        <v>51</v>
-      </c>
-      <c r="H5" s="2">
-        <v>6</v>
-      </c>
-      <c r="I5" s="2">
-        <v>9</v>
-      </c>
-      <c r="J5" s="2">
-        <v>24</v>
-      </c>
-      <c r="K5" s="2">
-        <v>87</v>
-      </c>
-      <c r="L5" s="2">
-        <v>19</v>
-      </c>
-      <c r="M5" s="2">
-        <v>7</v>
-      </c>
-      <c r="N5" s="2">
-        <v>50</v>
-      </c>
-      <c r="O5" s="2">
-        <v>54</v>
-      </c>
-      <c r="P5" s="2">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>37</v>
-      </c>
-      <c r="R5" s="2">
-        <v>67</v>
-      </c>
-      <c r="S5" s="2">
-        <v>67</v>
-      </c>
-      <c r="T5" s="2">
-        <v>61</v>
-      </c>
-      <c r="U5" s="2">
-        <v>58</v>
-      </c>
-      <c r="V5" s="2">
-        <v>91</v>
-      </c>
-      <c r="W5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23">
-      <c r="A6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="2">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2">
-        <v>26</v>
-      </c>
-      <c r="D6" s="2">
-        <v>19</v>
-      </c>
-      <c r="E6" s="2">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2">
-        <v>27</v>
-      </c>
-      <c r="G6" s="2">
-        <v>31</v>
-      </c>
-      <c r="H6" s="2">
-        <v>42</v>
-      </c>
-      <c r="I6" s="2">
-        <v>16</v>
-      </c>
-      <c r="J6" s="2">
-        <v>-8</v>
-      </c>
-      <c r="K6" s="2">
-        <v>4</v>
-      </c>
-      <c r="L6" s="2">
-        <v>-36</v>
-      </c>
-      <c r="M6" s="2">
-        <v>16</v>
-      </c>
-      <c r="N6" s="2">
-        <v>27</v>
-      </c>
-      <c r="O6" s="2">
-        <v>24</v>
-      </c>
-      <c r="P6" s="2">
-        <v>35</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>23</v>
-      </c>
-      <c r="R6" s="2">
-        <v>46</v>
-      </c>
-      <c r="S6" s="2">
-        <v>5</v>
-      </c>
-      <c r="T6" s="2">
-        <v>27</v>
-      </c>
-      <c r="U6" s="2">
-        <v>29</v>
-      </c>
-      <c r="V6" s="2">
-        <v>43</v>
-      </c>
-      <c r="W6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23">
-      <c r="A7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="2">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2">
-        <v>47</v>
-      </c>
-      <c r="D7" s="2">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2">
-        <v>40</v>
-      </c>
-      <c r="F7" s="2">
-        <v>12</v>
-      </c>
-      <c r="G7" s="2">
-        <v>8</v>
-      </c>
-      <c r="H7" s="2">
-        <v>-13</v>
-      </c>
-      <c r="I7" s="2">
-        <v>25</v>
-      </c>
-      <c r="J7" s="2">
-        <v>6</v>
-      </c>
-      <c r="K7" s="2">
-        <v>22</v>
-      </c>
-      <c r="L7" s="2">
-        <v>37</v>
-      </c>
-      <c r="M7" s="2">
-        <v>25</v>
-      </c>
-      <c r="N7" s="2">
-        <v>15</v>
-      </c>
-      <c r="O7" s="2">
-        <v>-9</v>
-      </c>
-      <c r="P7" s="2">
-        <v>43</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>7</v>
-      </c>
-      <c r="R7" s="2">
-        <v>13</v>
-      </c>
-      <c r="S7" s="2">
-        <v>15</v>
-      </c>
-      <c r="T7" s="2">
-        <v>13</v>
-      </c>
-      <c r="U7" s="2">
-        <v>45</v>
-      </c>
-      <c r="V7" s="2">
-        <v>60</v>
-      </c>
-      <c r="W7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23">
-      <c r="A8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="2">
-        <v>-10</v>
-      </c>
-      <c r="C8" s="2">
-        <v>42</v>
-      </c>
-      <c r="D8" s="2">
-        <v>14</v>
-      </c>
-      <c r="E8" s="2">
-        <v>22</v>
-      </c>
-      <c r="F8" s="2">
-        <v>18</v>
-      </c>
-      <c r="G8" s="2">
-        <v>-6</v>
-      </c>
-      <c r="H8" s="2">
-        <v>24</v>
-      </c>
-      <c r="I8" s="2">
-        <v>31</v>
-      </c>
-      <c r="J8" s="2">
-        <v>35</v>
-      </c>
-      <c r="K8" s="2">
-        <v>-4</v>
-      </c>
-      <c r="L8" s="2">
-        <v>34</v>
-      </c>
-      <c r="M8" s="2">
-        <v>-35</v>
-      </c>
-      <c r="N8" s="2">
-        <v>17</v>
-      </c>
-      <c r="O8" s="2">
-        <v>29</v>
-      </c>
-      <c r="P8" s="2">
-        <v>38</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>27</v>
-      </c>
-      <c r="R8" s="2">
-        <v>41</v>
-      </c>
-      <c r="S8" s="2">
-        <v>16</v>
-      </c>
-      <c r="T8" s="2">
-        <v>34</v>
-      </c>
-      <c r="U8" s="2">
-        <v>-10</v>
-      </c>
-      <c r="V8" s="2">
-        <v>54</v>
-      </c>
-      <c r="W8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23">
-      <c r="A9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="2">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>-22</v>
-      </c>
-      <c r="F9" s="2">
-        <v>10</v>
-      </c>
-      <c r="G9" s="2">
-        <v>9</v>
-      </c>
-      <c r="H9" s="2">
-        <v>13</v>
-      </c>
-      <c r="I9" s="2">
-        <v>7</v>
-      </c>
-      <c r="J9" s="2">
-        <v>52</v>
-      </c>
-      <c r="K9" s="2">
-        <v>26</v>
-      </c>
-      <c r="L9" s="2">
-        <v>45</v>
-      </c>
-      <c r="M9" s="2">
-        <v>14</v>
-      </c>
-      <c r="N9" s="2">
-        <v>24</v>
-      </c>
-      <c r="O9" s="2">
-        <v>35</v>
-      </c>
-      <c r="P9" s="2">
-        <v>14</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>-2</v>
-      </c>
-      <c r="R9" s="2">
-        <v>17</v>
-      </c>
-      <c r="S9" s="2">
-        <v>-4</v>
-      </c>
-      <c r="T9" s="2">
-        <v>25</v>
-      </c>
-      <c r="U9" s="2">
-        <v>2</v>
-      </c>
-      <c r="V9" s="2">
-        <v>-14</v>
-      </c>
-      <c r="W9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23">
-      <c r="A10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2">
-        <v>9</v>
-      </c>
-      <c r="E10" s="2">
-        <v>18</v>
-      </c>
-      <c r="F10" s="2">
-        <v>11</v>
-      </c>
-      <c r="G10" s="2">
-        <v>13</v>
-      </c>
-      <c r="H10" s="2">
-        <v>14</v>
-      </c>
-      <c r="I10" s="2">
-        <v>-4</v>
-      </c>
-      <c r="J10" s="2">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2">
-        <v>31</v>
-      </c>
-      <c r="L10" s="2">
-        <v>24</v>
-      </c>
-      <c r="M10" s="2">
-        <v>33</v>
-      </c>
-      <c r="N10" s="2">
-        <v>20</v>
-      </c>
-      <c r="O10" s="2">
-        <v>45</v>
-      </c>
-      <c r="P10" s="2">
-        <v>41</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>-11</v>
-      </c>
-      <c r="R10" s="2">
-        <v>-2</v>
-      </c>
-      <c r="S10" s="2">
-        <v>37</v>
-      </c>
-      <c r="T10" s="2">
-        <v>-12</v>
-      </c>
-      <c r="U10" s="2">
-        <v>2</v>
-      </c>
-      <c r="V10" s="2">
-        <v>8</v>
-      </c>
-      <c r="W10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23">
-      <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2">
-        <v>-14</v>
-      </c>
-      <c r="C11" s="2">
-        <v>-6</v>
-      </c>
-      <c r="D11" s="2">
-        <v>9</v>
-      </c>
-      <c r="E11" s="2">
-        <v>22</v>
-      </c>
-      <c r="F11" s="2">
-        <v>-6</v>
-      </c>
-      <c r="G11" s="2">
-        <v>10</v>
-      </c>
-      <c r="H11" s="2">
-        <v>10</v>
-      </c>
-      <c r="I11" s="2">
-        <v>-11</v>
-      </c>
-      <c r="J11" s="2">
-        <v>31</v>
-      </c>
-      <c r="K11" s="2">
-        <v>11</v>
-      </c>
-      <c r="L11" s="2">
-        <v>17</v>
-      </c>
-      <c r="M11" s="2">
-        <v>5</v>
-      </c>
-      <c r="N11" s="2">
-        <v>-13</v>
-      </c>
-      <c r="O11" s="2">
-        <v>2</v>
-      </c>
-      <c r="P11" s="2">
-        <v>14</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>6</v>
-      </c>
-      <c r="R11" s="2">
-        <v>7</v>
-      </c>
-      <c r="S11" s="2">
-        <v>6</v>
-      </c>
-      <c r="T11" s="2">
-        <v>18</v>
-      </c>
-      <c r="U11" s="2">
-        <v>14</v>
-      </c>
-      <c r="V11" s="2">
-        <v>14</v>
-      </c>
-      <c r="W11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED373387-C4B1-4C53-B689-3A35B6C15A04}">
-  <dimension ref="A1:X24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X2" sqref="X2"/>
+      <selection pane="bottomRight" activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3015,6 +2213,841 @@
   <sheetData>
     <row r="1" spans="1:24" s="4" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2">
+        <v>71</v>
+      </c>
+      <c r="C2" s="2">
+        <v>101</v>
+      </c>
+      <c r="D2" s="2">
+        <v>71</v>
+      </c>
+      <c r="E2" s="2">
+        <v>92</v>
+      </c>
+      <c r="F2" s="2">
+        <v>86</v>
+      </c>
+      <c r="G2" s="2">
+        <v>118</v>
+      </c>
+      <c r="H2" s="2">
+        <v>82</v>
+      </c>
+      <c r="I2" s="2">
+        <v>83</v>
+      </c>
+      <c r="J2" s="2">
+        <v>88</v>
+      </c>
+      <c r="K2" s="2">
+        <v>40</v>
+      </c>
+      <c r="L2" s="2">
+        <v>100</v>
+      </c>
+      <c r="M2" s="2">
+        <v>90</v>
+      </c>
+      <c r="N2" s="2">
+        <v>93</v>
+      </c>
+      <c r="O2" s="2">
+        <v>100</v>
+      </c>
+      <c r="P2" s="2">
+        <v>52</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>97</v>
+      </c>
+      <c r="R2" s="2">
+        <v>6</v>
+      </c>
+      <c r="S2" s="2">
+        <v>64</v>
+      </c>
+      <c r="T2" s="2">
+        <v>22</v>
+      </c>
+      <c r="U2" s="2">
+        <v>86</v>
+      </c>
+      <c r="V2" s="2">
+        <v>63</v>
+      </c>
+      <c r="W2" s="2">
+        <v>-34</v>
+      </c>
+      <c r="X2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-23</v>
+      </c>
+      <c r="D3" s="2">
+        <v>56</v>
+      </c>
+      <c r="E3" s="2">
+        <v>73</v>
+      </c>
+      <c r="F3" s="2">
+        <v>64</v>
+      </c>
+      <c r="G3" s="2">
+        <v>34</v>
+      </c>
+      <c r="H3" s="2">
+        <v>67</v>
+      </c>
+      <c r="I3" s="2">
+        <v>71</v>
+      </c>
+      <c r="J3" s="2">
+        <v>61</v>
+      </c>
+      <c r="K3" s="2">
+        <v>57</v>
+      </c>
+      <c r="L3" s="2">
+        <v>67</v>
+      </c>
+      <c r="M3" s="2">
+        <v>41</v>
+      </c>
+      <c r="N3" s="2">
+        <v>70</v>
+      </c>
+      <c r="O3" s="2">
+        <v>39</v>
+      </c>
+      <c r="P3" s="2">
+        <v>-4</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>67</v>
+      </c>
+      <c r="R3" s="2">
+        <v>28</v>
+      </c>
+      <c r="S3" s="2">
+        <v>48</v>
+      </c>
+      <c r="T3" s="2">
+        <v>85</v>
+      </c>
+      <c r="U3" s="2">
+        <v>58</v>
+      </c>
+      <c r="V3" s="2">
+        <v>-3</v>
+      </c>
+      <c r="W3" s="2">
+        <v>48</v>
+      </c>
+      <c r="X3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2">
+        <v>67</v>
+      </c>
+      <c r="D4" s="2">
+        <v>46</v>
+      </c>
+      <c r="E4" s="2">
+        <v>46</v>
+      </c>
+      <c r="F4" s="2">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2">
+        <v>60</v>
+      </c>
+      <c r="H4" s="2">
+        <v>71</v>
+      </c>
+      <c r="I4" s="2">
+        <v>23</v>
+      </c>
+      <c r="J4" s="2">
+        <v>28</v>
+      </c>
+      <c r="K4" s="2">
+        <v>51</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>41</v>
+      </c>
+      <c r="N4" s="2">
+        <v>55</v>
+      </c>
+      <c r="O4" s="2">
+        <v>39</v>
+      </c>
+      <c r="P4" s="2">
+        <v>47</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>56</v>
+      </c>
+      <c r="R4" s="2">
+        <v>85</v>
+      </c>
+      <c r="S4" s="2">
+        <v>51</v>
+      </c>
+      <c r="T4" s="2">
+        <v>92</v>
+      </c>
+      <c r="U4" s="2">
+        <v>36</v>
+      </c>
+      <c r="V4" s="2">
+        <v>88</v>
+      </c>
+      <c r="W4" s="2">
+        <v>85</v>
+      </c>
+      <c r="X4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2">
+        <v>67</v>
+      </c>
+      <c r="C5" s="2">
+        <v>69</v>
+      </c>
+      <c r="D5" s="2">
+        <v>56</v>
+      </c>
+      <c r="E5" s="2">
+        <v>60</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46</v>
+      </c>
+      <c r="G5" s="2">
+        <v>51</v>
+      </c>
+      <c r="H5" s="2">
+        <v>6</v>
+      </c>
+      <c r="I5" s="2">
+        <v>9</v>
+      </c>
+      <c r="J5" s="2">
+        <v>24</v>
+      </c>
+      <c r="K5" s="2">
+        <v>87</v>
+      </c>
+      <c r="L5" s="2">
+        <v>19</v>
+      </c>
+      <c r="M5" s="2">
+        <v>7</v>
+      </c>
+      <c r="N5" s="2">
+        <v>50</v>
+      </c>
+      <c r="O5" s="2">
+        <v>54</v>
+      </c>
+      <c r="P5" s="2">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>37</v>
+      </c>
+      <c r="R5" s="2">
+        <v>67</v>
+      </c>
+      <c r="S5" s="2">
+        <v>67</v>
+      </c>
+      <c r="T5" s="2">
+        <v>61</v>
+      </c>
+      <c r="U5" s="2">
+        <v>58</v>
+      </c>
+      <c r="V5" s="2">
+        <v>91</v>
+      </c>
+      <c r="W5" s="2">
+        <v>77</v>
+      </c>
+      <c r="X5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="2">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2">
+        <v>27</v>
+      </c>
+      <c r="G6" s="2">
+        <v>31</v>
+      </c>
+      <c r="H6" s="2">
+        <v>42</v>
+      </c>
+      <c r="I6" s="2">
+        <v>16</v>
+      </c>
+      <c r="J6" s="2">
+        <v>-8</v>
+      </c>
+      <c r="K6" s="2">
+        <v>4</v>
+      </c>
+      <c r="L6" s="2">
+        <v>-36</v>
+      </c>
+      <c r="M6" s="2">
+        <v>16</v>
+      </c>
+      <c r="N6" s="2">
+        <v>27</v>
+      </c>
+      <c r="O6" s="2">
+        <v>24</v>
+      </c>
+      <c r="P6" s="2">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>23</v>
+      </c>
+      <c r="R6" s="2">
+        <v>46</v>
+      </c>
+      <c r="S6" s="2">
+        <v>5</v>
+      </c>
+      <c r="T6" s="2">
+        <v>27</v>
+      </c>
+      <c r="U6" s="2">
+        <v>29</v>
+      </c>
+      <c r="V6" s="2">
+        <v>42</v>
+      </c>
+      <c r="W6" s="2">
+        <v>9</v>
+      </c>
+      <c r="X6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2">
+        <v>47</v>
+      </c>
+      <c r="D7" s="2">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2">
+        <v>40</v>
+      </c>
+      <c r="F7" s="2">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2">
+        <v>-13</v>
+      </c>
+      <c r="I7" s="2">
+        <v>25</v>
+      </c>
+      <c r="J7" s="2">
+        <v>6</v>
+      </c>
+      <c r="K7" s="2">
+        <v>22</v>
+      </c>
+      <c r="L7" s="2">
+        <v>37</v>
+      </c>
+      <c r="M7" s="2">
+        <v>25</v>
+      </c>
+      <c r="N7" s="2">
+        <v>15</v>
+      </c>
+      <c r="O7" s="2">
+        <v>-9</v>
+      </c>
+      <c r="P7" s="2">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>7</v>
+      </c>
+      <c r="R7" s="2">
+        <v>13</v>
+      </c>
+      <c r="S7" s="2">
+        <v>15</v>
+      </c>
+      <c r="T7" s="2">
+        <v>13</v>
+      </c>
+      <c r="U7" s="2">
+        <v>45</v>
+      </c>
+      <c r="V7" s="2">
+        <v>54</v>
+      </c>
+      <c r="W7" s="2">
+        <v>24</v>
+      </c>
+      <c r="X7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-10</v>
+      </c>
+      <c r="C8" s="2">
+        <v>42</v>
+      </c>
+      <c r="D8" s="2">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2">
+        <v>22</v>
+      </c>
+      <c r="F8" s="2">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-6</v>
+      </c>
+      <c r="H8" s="2">
+        <v>24</v>
+      </c>
+      <c r="I8" s="2">
+        <v>31</v>
+      </c>
+      <c r="J8" s="2">
+        <v>35</v>
+      </c>
+      <c r="K8" s="2">
+        <v>-4</v>
+      </c>
+      <c r="L8" s="2">
+        <v>34</v>
+      </c>
+      <c r="M8" s="2">
+        <v>-35</v>
+      </c>
+      <c r="N8" s="2">
+        <v>17</v>
+      </c>
+      <c r="O8" s="2">
+        <v>29</v>
+      </c>
+      <c r="P8" s="2">
+        <v>38</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>27</v>
+      </c>
+      <c r="R8" s="2">
+        <v>41</v>
+      </c>
+      <c r="S8" s="2">
+        <v>16</v>
+      </c>
+      <c r="T8" s="2">
+        <v>34</v>
+      </c>
+      <c r="U8" s="2">
+        <v>-10</v>
+      </c>
+      <c r="V8" s="2">
+        <v>47</v>
+      </c>
+      <c r="W8" s="2">
+        <v>30</v>
+      </c>
+      <c r="X8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>-22</v>
+      </c>
+      <c r="F9" s="2">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2">
+        <v>9</v>
+      </c>
+      <c r="H9" s="2">
+        <v>13</v>
+      </c>
+      <c r="I9" s="2">
+        <v>7</v>
+      </c>
+      <c r="J9" s="2">
+        <v>52</v>
+      </c>
+      <c r="K9" s="2">
+        <v>26</v>
+      </c>
+      <c r="L9" s="2">
+        <v>45</v>
+      </c>
+      <c r="M9" s="2">
+        <v>14</v>
+      </c>
+      <c r="N9" s="2">
+        <v>24</v>
+      </c>
+      <c r="O9" s="2">
+        <v>35</v>
+      </c>
+      <c r="P9" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>-2</v>
+      </c>
+      <c r="R9" s="2">
+        <v>17</v>
+      </c>
+      <c r="S9" s="2">
+        <v>-4</v>
+      </c>
+      <c r="T9" s="2">
+        <v>25</v>
+      </c>
+      <c r="U9" s="2">
+        <v>2</v>
+      </c>
+      <c r="V9" s="2">
+        <v>-14</v>
+      </c>
+      <c r="W9" s="2">
+        <v>0</v>
+      </c>
+      <c r="X9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2">
+        <v>18</v>
+      </c>
+      <c r="F10" s="2">
+        <v>11</v>
+      </c>
+      <c r="G10" s="2">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2">
+        <v>14</v>
+      </c>
+      <c r="I10" s="2">
+        <v>-4</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>31</v>
+      </c>
+      <c r="L10" s="2">
+        <v>24</v>
+      </c>
+      <c r="M10" s="2">
+        <v>33</v>
+      </c>
+      <c r="N10" s="2">
+        <v>20</v>
+      </c>
+      <c r="O10" s="2">
+        <v>45</v>
+      </c>
+      <c r="P10" s="2">
+        <v>41</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>-11</v>
+      </c>
+      <c r="R10" s="2">
+        <v>-2</v>
+      </c>
+      <c r="S10" s="2">
+        <v>37</v>
+      </c>
+      <c r="T10" s="2">
+        <v>-12</v>
+      </c>
+      <c r="U10" s="2">
+        <v>2</v>
+      </c>
+      <c r="V10" s="2">
+        <v>-9</v>
+      </c>
+      <c r="W10" s="2">
+        <v>-8</v>
+      </c>
+      <c r="X10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2">
+        <v>-14</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>9</v>
+      </c>
+      <c r="E11" s="2">
+        <v>22</v>
+      </c>
+      <c r="F11" s="2">
+        <v>-6</v>
+      </c>
+      <c r="G11" s="2">
+        <v>10</v>
+      </c>
+      <c r="H11" s="2">
+        <v>10</v>
+      </c>
+      <c r="I11" s="2">
+        <v>-11</v>
+      </c>
+      <c r="J11" s="2">
+        <v>31</v>
+      </c>
+      <c r="K11" s="2">
+        <v>11</v>
+      </c>
+      <c r="L11" s="2">
+        <v>17</v>
+      </c>
+      <c r="M11" s="2">
+        <v>5</v>
+      </c>
+      <c r="N11" s="2">
+        <v>-13</v>
+      </c>
+      <c r="O11" s="2">
+        <v>2</v>
+      </c>
+      <c r="P11" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>6</v>
+      </c>
+      <c r="R11" s="2">
+        <v>7</v>
+      </c>
+      <c r="S11" s="2">
+        <v>6</v>
+      </c>
+      <c r="T11" s="2">
+        <v>18</v>
+      </c>
+      <c r="U11" s="2">
+        <v>14</v>
+      </c>
+      <c r="V11" s="2">
+        <v>12</v>
+      </c>
+      <c r="W11" s="2">
+        <v>3</v>
+      </c>
+      <c r="X11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED373387-C4B1-4C53-B689-3A35B6C15A04}">
+  <dimension ref="A1:Y24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="Y23" sqref="Y23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A1" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -3086,8 +3119,11 @@
       <c r="X1" s="3">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:24">
+      <c r="Y1" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -3160,8 +3196,11 @@
       <c r="X2" s="2">
         <v>30.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="Y2" s="2">
+        <v>30.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -3234,8 +3273,11 @@
       <c r="X3" s="2">
         <v>29.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="Y3" s="2">
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3308,8 +3350,11 @@
       <c r="X4" s="2">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="Y4" s="2">
+        <v>25.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -3382,8 +3427,11 @@
       <c r="X5" s="2">
         <v>23.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="Y5" s="2">
+        <v>23.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -3456,8 +3504,11 @@
       <c r="X6" s="2">
         <v>22.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="Y6" s="2">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -3530,8 +3581,11 @@
       <c r="X7" s="2">
         <v>23.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="Y7" s="2">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -3564,8 +3618,9 @@
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="Y8" s="2"/>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
@@ -3638,8 +3693,11 @@
       <c r="X9" s="2">
         <v>16.899999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:24">
+      <c r="Y9" s="2">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -3708,8 +3766,11 @@
       <c r="X10" s="2">
         <v>11.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="Y10" s="2">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -3782,8 +3843,11 @@
       <c r="X11" s="2">
         <v>13.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:24">
+      <c r="Y11" s="2">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -3816,8 +3880,9 @@
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
-    </row>
-    <row r="13" spans="1:24">
+      <c r="Y12" s="2"/>
+    </row>
+    <row r="13" spans="1:25">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -3890,8 +3955,11 @@
       <c r="X13" s="2">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="14" spans="1:24">
+      <c r="Y13" s="2">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -3964,8 +4032,11 @@
       <c r="X14" s="2">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:24">
+      <c r="Y14" s="2">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -4038,8 +4109,11 @@
       <c r="X15" s="2">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="16" spans="1:24">
+      <c r="Y15" s="2">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -4112,8 +4186,11 @@
       <c r="X16" s="2">
         <v>6.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:24">
+      <c r="Y16" s="2">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -4186,8 +4263,11 @@
       <c r="X17" s="2">
         <v>8.9</v>
       </c>
-    </row>
-    <row r="18" spans="1:24">
+      <c r="Y17" s="2">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
@@ -4260,8 +4340,11 @@
       <c r="X18" s="2">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:24">
+      <c r="Y18" s="2">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
       <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
@@ -4334,8 +4417,11 @@
       <c r="X19" s="2">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:24">
+      <c r="Y19" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
@@ -4376,8 +4462,9 @@
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
-    </row>
-    <row r="21" spans="1:24">
+      <c r="Y20" s="2"/>
+    </row>
+    <row r="21" spans="1:25">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
@@ -4450,8 +4537,11 @@
       <c r="X21" s="2">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="22" spans="1:24">
+      <c r="Y21" s="2">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -4518,10 +4608,13 @@
         <v>6.5</v>
       </c>
       <c r="X22" s="2">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24">
+        <v>5.9</v>
+      </c>
+      <c r="Y22" s="2">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
       <c r="A23" s="2" t="s">
         <v>39</v>
       </c>
@@ -4594,8 +4687,11 @@
       <c r="X23" s="2">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="24" spans="1:24">
+      <c r="Y23" s="2">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -4656,6 +4752,9 @@
       <c r="X24" s="2">
         <v>4.5</v>
       </c>
+      <c r="Y24" s="2">
+        <v>4.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4664,13 +4763,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C15A70-BFDE-46F9-9F77-0BE1119DCB97}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U22" sqref="U22"/>
+      <selection pane="bottomRight" activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4678,7 +4777,7 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:24" s="4" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>41</v>
       </c>
@@ -4748,8 +4847,11 @@
       <c r="W1" s="3">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:23">
+      <c r="X1" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -4819,8 +4921,11 @@
       <c r="W2" s="2">
         <v>35.9</v>
       </c>
-    </row>
-    <row r="3" spans="1:23">
+      <c r="X2" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -4890,8 +4995,11 @@
       <c r="W3" s="2">
         <v>31.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:23">
+      <c r="X3" s="2">
+        <v>31.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -4961,8 +5069,11 @@
       <c r="W4" s="2">
         <v>30.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:23">
+      <c r="X4" s="2">
+        <v>30.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -5032,8 +5143,11 @@
       <c r="W5" s="2">
         <v>27.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:23">
+      <c r="X5" s="2">
+        <v>28.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -5103,8 +5217,11 @@
       <c r="W6" s="2">
         <v>18.899999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:23">
+      <c r="X6" s="2">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
@@ -5174,8 +5291,11 @@
       <c r="W7" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:23">
+      <c r="X7" s="2">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -5245,8 +5365,11 @@
       <c r="W8" s="2">
         <v>14.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:23">
+      <c r="X8" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -5316,8 +5439,11 @@
       <c r="W9" s="2">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:23">
+      <c r="X9" s="2">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -5387,8 +5513,11 @@
       <c r="W10" s="2">
         <v>9.6999999999999993</v>
       </c>
-    </row>
-    <row r="11" spans="1:23">
+      <c r="X10" s="2">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -5457,6 +5586,9 @@
       </c>
       <c r="W11" s="2">
         <v>9.9</v>
+      </c>
+      <c r="X11" s="2">
+        <v>9.3000000000000007</v>
       </c>
     </row>
   </sheetData>
@@ -14163,13 +14295,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11985E4F-6F4E-4304-AF61-8A6F49D5D125}">
-  <dimension ref="A1:X24"/>
+  <dimension ref="A1:Y24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC22" sqref="AC22"/>
+      <selection pane="bottomRight" activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14177,7 +14309,7 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="4" customFormat="1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:25" s="4" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>40</v>
       </c>
@@ -14250,8 +14382,11 @@
       <c r="X1" s="3">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:24">
+      <c r="Y1" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -14322,10 +14457,13 @@
         <v>49</v>
       </c>
       <c r="X2" s="2">
+        <v>-10</v>
+      </c>
+      <c r="Y2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -14396,10 +14534,13 @@
         <v>-1</v>
       </c>
       <c r="X3" s="2">
+        <v>-14</v>
+      </c>
+      <c r="Y3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -14467,13 +14608,16 @@
         <v>26</v>
       </c>
       <c r="W4" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="X4" s="2">
+        <v>56</v>
+      </c>
+      <c r="Y4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -14544,10 +14688,13 @@
         <v>31</v>
       </c>
       <c r="X5" s="2">
+        <v>30</v>
+      </c>
+      <c r="Y5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -14618,10 +14765,13 @@
         <v>-11</v>
       </c>
       <c r="X6" s="2">
+        <v>18</v>
+      </c>
+      <c r="Y6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -14689,13 +14839,16 @@
         <v>29</v>
       </c>
       <c r="W7" s="2">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="X7" s="2">
+        <v>23</v>
+      </c>
+      <c r="Y7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:25">
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
@@ -14766,10 +14919,13 @@
         <v>40</v>
       </c>
       <c r="X8" s="2">
+        <v>32</v>
+      </c>
+      <c r="Y8" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -14840,10 +14996,13 @@
         <v>19</v>
       </c>
       <c r="X9" s="2">
+        <v>-17</v>
+      </c>
+      <c r="Y9" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:25">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -14911,13 +15070,16 @@
         <v>36</v>
       </c>
       <c r="W10" s="2">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="X10" s="2">
+        <v>10</v>
+      </c>
+      <c r="Y10" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -14981,13 +15143,16 @@
         <v>3</v>
       </c>
       <c r="W11" s="2">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="X11" s="2">
+        <v>9</v>
+      </c>
+      <c r="Y11" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -15055,13 +15220,16 @@
         <v>14</v>
       </c>
       <c r="W12" s="2">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="X12" s="2">
+        <v>-20</v>
+      </c>
+      <c r="Y12" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -15132,10 +15300,13 @@
         <v>5</v>
       </c>
       <c r="X13" s="2">
+        <v>11</v>
+      </c>
+      <c r="Y13" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:25">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -15206,10 +15377,13 @@
         <v>17</v>
       </c>
       <c r="X14" s="2">
+        <v>9</v>
+      </c>
+      <c r="Y14" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:25">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
@@ -15277,13 +15451,16 @@
         <v>-2</v>
       </c>
       <c r="W15" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="X15" s="2">
+        <v>16</v>
+      </c>
+      <c r="Y15" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:25">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -15354,10 +15531,13 @@
         <v>-24</v>
       </c>
       <c r="X16" s="2">
+        <v>-20</v>
+      </c>
+      <c r="Y16" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -15425,13 +15605,16 @@
         <v>6</v>
       </c>
       <c r="W17" s="2">
+        <v>15</v>
+      </c>
+      <c r="X17" s="2">
         <v>16</v>
       </c>
-      <c r="X17" s="2">
+      <c r="Y17" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:25">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -15464,8 +15647,9 @@
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
-    </row>
-    <row r="19" spans="1:24">
+      <c r="Y18" s="2"/>
+    </row>
+    <row r="19" spans="1:25">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -15498,8 +15682,9 @@
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
-    </row>
-    <row r="20" spans="1:24">
+      <c r="Y19" s="2"/>
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -15563,13 +15748,16 @@
         <v>-18</v>
       </c>
       <c r="W20" s="2">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="X20" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Y20" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -15637,13 +15825,16 @@
         <v>9</v>
       </c>
       <c r="W21" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="X21" s="2">
+        <v>-2</v>
+      </c>
+      <c r="Y21" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:25">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -15704,8 +15895,11 @@
       <c r="X22" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:24">
+      <c r="Y22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
       <c r="A23" s="2" t="s">
         <v>4</v>
       </c>
@@ -15776,10 +15970,13 @@
         <v>2</v>
       </c>
       <c r="X23" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y23" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:25">
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Latest points, changed cumulative method
</commit_message>
<xml_diff>
--- a/data/f1_fantasy_archive.xlsx
+++ b/data/f1_fantasy_archive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexs\Dropbox\Dev\f1_fantasy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77149FA0-1509-474A-89AC-C5A0FAC330E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96832963-A2D1-4204-ADF4-57C0CC6E881F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="8" xr2:uid="{5075C4C2-DC0E-48A5-BDF1-482703F248E6}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="10" activeTab="11" xr2:uid="{5075C4C2-DC0E-48A5-BDF1-482703F248E6}"/>
   </bookViews>
   <sheets>
     <sheet name="2023 Drivers Points" sheetId="1" r:id="rId1"/>
@@ -2197,848 +2197,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2707B16-05A3-42D1-BE37-AF149E8BEDBE}">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V14" sqref="V14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" s="4" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="3">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3">
-        <v>16</v>
-      </c>
-      <c r="R1" s="3">
-        <v>17</v>
-      </c>
-      <c r="S1" s="3">
-        <v>18</v>
-      </c>
-      <c r="T1" s="3">
-        <v>19</v>
-      </c>
-      <c r="U1" s="3">
-        <v>20</v>
-      </c>
-      <c r="V1" s="3">
-        <v>21</v>
-      </c>
-      <c r="W1" s="3">
-        <v>22</v>
-      </c>
-      <c r="X1" s="3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2">
-        <v>71</v>
-      </c>
-      <c r="C2" s="2">
-        <v>101</v>
-      </c>
-      <c r="D2" s="2">
-        <v>71</v>
-      </c>
-      <c r="E2" s="2">
-        <v>92</v>
-      </c>
-      <c r="F2" s="2">
-        <v>86</v>
-      </c>
-      <c r="G2" s="2">
-        <v>118</v>
-      </c>
-      <c r="H2" s="2">
-        <v>82</v>
-      </c>
-      <c r="I2" s="2">
-        <v>83</v>
-      </c>
-      <c r="J2" s="2">
-        <v>88</v>
-      </c>
-      <c r="K2" s="2">
-        <v>40</v>
-      </c>
-      <c r="L2" s="2">
-        <v>100</v>
-      </c>
-      <c r="M2" s="2">
-        <v>90</v>
-      </c>
-      <c r="N2" s="2">
-        <v>93</v>
-      </c>
-      <c r="O2" s="2">
-        <v>100</v>
-      </c>
-      <c r="P2" s="2">
-        <v>52</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>97</v>
-      </c>
-      <c r="R2" s="2">
-        <v>6</v>
-      </c>
-      <c r="S2" s="2">
-        <v>64</v>
-      </c>
-      <c r="T2" s="2">
-        <v>22</v>
-      </c>
-      <c r="U2" s="2">
-        <v>86</v>
-      </c>
-      <c r="V2" s="2">
-        <v>63</v>
-      </c>
-      <c r="W2" s="2">
-        <v>-34</v>
-      </c>
-      <c r="X2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2">
-        <v>36</v>
-      </c>
-      <c r="C3" s="2">
-        <v>-23</v>
-      </c>
-      <c r="D3" s="2">
-        <v>56</v>
-      </c>
-      <c r="E3" s="2">
-        <v>73</v>
-      </c>
-      <c r="F3" s="2">
-        <v>64</v>
-      </c>
-      <c r="G3" s="2">
-        <v>34</v>
-      </c>
-      <c r="H3" s="2">
-        <v>67</v>
-      </c>
-      <c r="I3" s="2">
-        <v>71</v>
-      </c>
-      <c r="J3" s="2">
-        <v>61</v>
-      </c>
-      <c r="K3" s="2">
-        <v>57</v>
-      </c>
-      <c r="L3" s="2">
-        <v>67</v>
-      </c>
-      <c r="M3" s="2">
-        <v>41</v>
-      </c>
-      <c r="N3" s="2">
-        <v>70</v>
-      </c>
-      <c r="O3" s="2">
-        <v>39</v>
-      </c>
-      <c r="P3" s="2">
-        <v>-4</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>67</v>
-      </c>
-      <c r="R3" s="2">
-        <v>28</v>
-      </c>
-      <c r="S3" s="2">
-        <v>48</v>
-      </c>
-      <c r="T3" s="2">
-        <v>85</v>
-      </c>
-      <c r="U3" s="2">
-        <v>58</v>
-      </c>
-      <c r="V3" s="2">
-        <v>-3</v>
-      </c>
-      <c r="W3" s="2">
-        <v>48</v>
-      </c>
-      <c r="X3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="2">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2">
-        <v>67</v>
-      </c>
-      <c r="D4" s="2">
-        <v>46</v>
-      </c>
-      <c r="E4" s="2">
-        <v>46</v>
-      </c>
-      <c r="F4" s="2">
-        <v>21</v>
-      </c>
-      <c r="G4" s="2">
-        <v>60</v>
-      </c>
-      <c r="H4" s="2">
-        <v>71</v>
-      </c>
-      <c r="I4" s="2">
-        <v>23</v>
-      </c>
-      <c r="J4" s="2">
-        <v>28</v>
-      </c>
-      <c r="K4" s="2">
-        <v>51</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2">
-        <v>41</v>
-      </c>
-      <c r="N4" s="2">
-        <v>55</v>
-      </c>
-      <c r="O4" s="2">
-        <v>39</v>
-      </c>
-      <c r="P4" s="2">
-        <v>47</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>56</v>
-      </c>
-      <c r="R4" s="2">
-        <v>85</v>
-      </c>
-      <c r="S4" s="2">
-        <v>51</v>
-      </c>
-      <c r="T4" s="2">
-        <v>92</v>
-      </c>
-      <c r="U4" s="2">
-        <v>36</v>
-      </c>
-      <c r="V4" s="2">
-        <v>88</v>
-      </c>
-      <c r="W4" s="2">
-        <v>85</v>
-      </c>
-      <c r="X4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24">
-      <c r="A5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="2">
-        <v>67</v>
-      </c>
-      <c r="C5" s="2">
-        <v>69</v>
-      </c>
-      <c r="D5" s="2">
-        <v>56</v>
-      </c>
-      <c r="E5" s="2">
-        <v>60</v>
-      </c>
-      <c r="F5" s="2">
-        <v>46</v>
-      </c>
-      <c r="G5" s="2">
-        <v>51</v>
-      </c>
-      <c r="H5" s="2">
-        <v>6</v>
-      </c>
-      <c r="I5" s="2">
-        <v>9</v>
-      </c>
-      <c r="J5" s="2">
-        <v>24</v>
-      </c>
-      <c r="K5" s="2">
-        <v>87</v>
-      </c>
-      <c r="L5" s="2">
-        <v>19</v>
-      </c>
-      <c r="M5" s="2">
-        <v>7</v>
-      </c>
-      <c r="N5" s="2">
-        <v>50</v>
-      </c>
-      <c r="O5" s="2">
-        <v>54</v>
-      </c>
-      <c r="P5" s="2">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>37</v>
-      </c>
-      <c r="R5" s="2">
-        <v>67</v>
-      </c>
-      <c r="S5" s="2">
-        <v>67</v>
-      </c>
-      <c r="T5" s="2">
-        <v>61</v>
-      </c>
-      <c r="U5" s="2">
-        <v>58</v>
-      </c>
-      <c r="V5" s="2">
-        <v>91</v>
-      </c>
-      <c r="W5" s="2">
-        <v>77</v>
-      </c>
-      <c r="X5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
-      <c r="A6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="2">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2">
-        <v>26</v>
-      </c>
-      <c r="D6" s="2">
-        <v>19</v>
-      </c>
-      <c r="E6" s="2">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2">
-        <v>27</v>
-      </c>
-      <c r="G6" s="2">
-        <v>31</v>
-      </c>
-      <c r="H6" s="2">
-        <v>42</v>
-      </c>
-      <c r="I6" s="2">
-        <v>16</v>
-      </c>
-      <c r="J6" s="2">
-        <v>-8</v>
-      </c>
-      <c r="K6" s="2">
-        <v>4</v>
-      </c>
-      <c r="L6" s="2">
-        <v>-36</v>
-      </c>
-      <c r="M6" s="2">
-        <v>16</v>
-      </c>
-      <c r="N6" s="2">
-        <v>27</v>
-      </c>
-      <c r="O6" s="2">
-        <v>24</v>
-      </c>
-      <c r="P6" s="2">
-        <v>35</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>23</v>
-      </c>
-      <c r="R6" s="2">
-        <v>46</v>
-      </c>
-      <c r="S6" s="2">
-        <v>5</v>
-      </c>
-      <c r="T6" s="2">
-        <v>27</v>
-      </c>
-      <c r="U6" s="2">
-        <v>29</v>
-      </c>
-      <c r="V6" s="2">
-        <v>42</v>
-      </c>
-      <c r="W6" s="2">
-        <v>9</v>
-      </c>
-      <c r="X6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24">
-      <c r="A7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="2">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2">
-        <v>47</v>
-      </c>
-      <c r="D7" s="2">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2">
-        <v>40</v>
-      </c>
-      <c r="F7" s="2">
-        <v>12</v>
-      </c>
-      <c r="G7" s="2">
-        <v>8</v>
-      </c>
-      <c r="H7" s="2">
-        <v>-13</v>
-      </c>
-      <c r="I7" s="2">
-        <v>25</v>
-      </c>
-      <c r="J7" s="2">
-        <v>6</v>
-      </c>
-      <c r="K7" s="2">
-        <v>22</v>
-      </c>
-      <c r="L7" s="2">
-        <v>37</v>
-      </c>
-      <c r="M7" s="2">
-        <v>25</v>
-      </c>
-      <c r="N7" s="2">
-        <v>15</v>
-      </c>
-      <c r="O7" s="2">
-        <v>-9</v>
-      </c>
-      <c r="P7" s="2">
-        <v>43</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>7</v>
-      </c>
-      <c r="R7" s="2">
-        <v>13</v>
-      </c>
-      <c r="S7" s="2">
-        <v>15</v>
-      </c>
-      <c r="T7" s="2">
-        <v>13</v>
-      </c>
-      <c r="U7" s="2">
-        <v>45</v>
-      </c>
-      <c r="V7" s="2">
-        <v>54</v>
-      </c>
-      <c r="W7" s="2">
-        <v>24</v>
-      </c>
-      <c r="X7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
-      <c r="A8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="2">
-        <v>-10</v>
-      </c>
-      <c r="C8" s="2">
-        <v>42</v>
-      </c>
-      <c r="D8" s="2">
-        <v>14</v>
-      </c>
-      <c r="E8" s="2">
-        <v>22</v>
-      </c>
-      <c r="F8" s="2">
-        <v>18</v>
-      </c>
-      <c r="G8" s="2">
-        <v>-6</v>
-      </c>
-      <c r="H8" s="2">
-        <v>24</v>
-      </c>
-      <c r="I8" s="2">
-        <v>31</v>
-      </c>
-      <c r="J8" s="2">
-        <v>35</v>
-      </c>
-      <c r="K8" s="2">
-        <v>-4</v>
-      </c>
-      <c r="L8" s="2">
-        <v>34</v>
-      </c>
-      <c r="M8" s="2">
-        <v>-35</v>
-      </c>
-      <c r="N8" s="2">
-        <v>17</v>
-      </c>
-      <c r="O8" s="2">
-        <v>29</v>
-      </c>
-      <c r="P8" s="2">
-        <v>38</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>27</v>
-      </c>
-      <c r="R8" s="2">
-        <v>41</v>
-      </c>
-      <c r="S8" s="2">
-        <v>16</v>
-      </c>
-      <c r="T8" s="2">
-        <v>34</v>
-      </c>
-      <c r="U8" s="2">
-        <v>-10</v>
-      </c>
-      <c r="V8" s="2">
-        <v>47</v>
-      </c>
-      <c r="W8" s="2">
-        <v>30</v>
-      </c>
-      <c r="X8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
-      <c r="A9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="2">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>-22</v>
-      </c>
-      <c r="F9" s="2">
-        <v>10</v>
-      </c>
-      <c r="G9" s="2">
-        <v>9</v>
-      </c>
-      <c r="H9" s="2">
-        <v>13</v>
-      </c>
-      <c r="I9" s="2">
-        <v>7</v>
-      </c>
-      <c r="J9" s="2">
-        <v>52</v>
-      </c>
-      <c r="K9" s="2">
-        <v>26</v>
-      </c>
-      <c r="L9" s="2">
-        <v>45</v>
-      </c>
-      <c r="M9" s="2">
-        <v>14</v>
-      </c>
-      <c r="N9" s="2">
-        <v>24</v>
-      </c>
-      <c r="O9" s="2">
-        <v>35</v>
-      </c>
-      <c r="P9" s="2">
-        <v>14</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>-2</v>
-      </c>
-      <c r="R9" s="2">
-        <v>17</v>
-      </c>
-      <c r="S9" s="2">
-        <v>-4</v>
-      </c>
-      <c r="T9" s="2">
-        <v>25</v>
-      </c>
-      <c r="U9" s="2">
-        <v>2</v>
-      </c>
-      <c r="V9" s="2">
-        <v>-14</v>
-      </c>
-      <c r="W9" s="2">
-        <v>0</v>
-      </c>
-      <c r="X9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24">
-      <c r="A10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2">
-        <v>9</v>
-      </c>
-      <c r="E10" s="2">
-        <v>18</v>
-      </c>
-      <c r="F10" s="2">
-        <v>11</v>
-      </c>
-      <c r="G10" s="2">
-        <v>13</v>
-      </c>
-      <c r="H10" s="2">
-        <v>14</v>
-      </c>
-      <c r="I10" s="2">
-        <v>-4</v>
-      </c>
-      <c r="J10" s="2">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2">
-        <v>31</v>
-      </c>
-      <c r="L10" s="2">
-        <v>24</v>
-      </c>
-      <c r="M10" s="2">
-        <v>33</v>
-      </c>
-      <c r="N10" s="2">
-        <v>20</v>
-      </c>
-      <c r="O10" s="2">
-        <v>45</v>
-      </c>
-      <c r="P10" s="2">
-        <v>41</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>-11</v>
-      </c>
-      <c r="R10" s="2">
-        <v>-2</v>
-      </c>
-      <c r="S10" s="2">
-        <v>37</v>
-      </c>
-      <c r="T10" s="2">
-        <v>-12</v>
-      </c>
-      <c r="U10" s="2">
-        <v>2</v>
-      </c>
-      <c r="V10" s="2">
-        <v>-9</v>
-      </c>
-      <c r="W10" s="2">
-        <v>-8</v>
-      </c>
-      <c r="X10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24">
-      <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2">
-        <v>-14</v>
-      </c>
-      <c r="C11" s="2">
-        <v>-6</v>
-      </c>
-      <c r="D11" s="2">
-        <v>9</v>
-      </c>
-      <c r="E11" s="2">
-        <v>22</v>
-      </c>
-      <c r="F11" s="2">
-        <v>-6</v>
-      </c>
-      <c r="G11" s="2">
-        <v>10</v>
-      </c>
-      <c r="H11" s="2">
-        <v>10</v>
-      </c>
-      <c r="I11" s="2">
-        <v>-11</v>
-      </c>
-      <c r="J11" s="2">
-        <v>31</v>
-      </c>
-      <c r="K11" s="2">
-        <v>11</v>
-      </c>
-      <c r="L11" s="2">
-        <v>17</v>
-      </c>
-      <c r="M11" s="2">
-        <v>5</v>
-      </c>
-      <c r="N11" s="2">
-        <v>-13</v>
-      </c>
-      <c r="O11" s="2">
-        <v>2</v>
-      </c>
-      <c r="P11" s="2">
-        <v>14</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>6</v>
-      </c>
-      <c r="R11" s="2">
-        <v>7</v>
-      </c>
-      <c r="S11" s="2">
-        <v>6</v>
-      </c>
-      <c r="T11" s="2">
-        <v>18</v>
-      </c>
-      <c r="U11" s="2">
-        <v>14</v>
-      </c>
-      <c r="V11" s="2">
-        <v>12</v>
-      </c>
-      <c r="W11" s="2">
-        <v>3</v>
-      </c>
-      <c r="X11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED373387-C4B1-4C53-B689-3A35B6C15A04}">
-  <dimension ref="A1:Y24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y23" sqref="Y23"/>
+      <selection pane="bottomRight" activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3048,6 +2213,874 @@
   <sheetData>
     <row r="1" spans="1:25" s="4" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2">
+        <v>71</v>
+      </c>
+      <c r="C2" s="2">
+        <v>101</v>
+      </c>
+      <c r="D2" s="2">
+        <v>71</v>
+      </c>
+      <c r="E2" s="2">
+        <v>92</v>
+      </c>
+      <c r="F2" s="2">
+        <v>86</v>
+      </c>
+      <c r="G2" s="2">
+        <v>118</v>
+      </c>
+      <c r="H2" s="2">
+        <v>82</v>
+      </c>
+      <c r="I2" s="2">
+        <v>83</v>
+      </c>
+      <c r="J2" s="2">
+        <v>88</v>
+      </c>
+      <c r="K2" s="2">
+        <v>40</v>
+      </c>
+      <c r="L2" s="2">
+        <v>100</v>
+      </c>
+      <c r="M2" s="2">
+        <v>90</v>
+      </c>
+      <c r="N2" s="2">
+        <v>93</v>
+      </c>
+      <c r="O2" s="2">
+        <v>100</v>
+      </c>
+      <c r="P2" s="2">
+        <v>52</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>97</v>
+      </c>
+      <c r="R2" s="2">
+        <v>6</v>
+      </c>
+      <c r="S2" s="2">
+        <v>64</v>
+      </c>
+      <c r="T2" s="2">
+        <v>22</v>
+      </c>
+      <c r="U2" s="2">
+        <v>86</v>
+      </c>
+      <c r="V2" s="2">
+        <v>63</v>
+      </c>
+      <c r="W2" s="2">
+        <v>-34</v>
+      </c>
+      <c r="X2" s="2">
+        <v>96</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-23</v>
+      </c>
+      <c r="D3" s="2">
+        <v>56</v>
+      </c>
+      <c r="E3" s="2">
+        <v>73</v>
+      </c>
+      <c r="F3" s="2">
+        <v>64</v>
+      </c>
+      <c r="G3" s="2">
+        <v>34</v>
+      </c>
+      <c r="H3" s="2">
+        <v>67</v>
+      </c>
+      <c r="I3" s="2">
+        <v>71</v>
+      </c>
+      <c r="J3" s="2">
+        <v>61</v>
+      </c>
+      <c r="K3" s="2">
+        <v>57</v>
+      </c>
+      <c r="L3" s="2">
+        <v>67</v>
+      </c>
+      <c r="M3" s="2">
+        <v>41</v>
+      </c>
+      <c r="N3" s="2">
+        <v>70</v>
+      </c>
+      <c r="O3" s="2">
+        <v>39</v>
+      </c>
+      <c r="P3" s="2">
+        <v>-4</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>67</v>
+      </c>
+      <c r="R3" s="2">
+        <v>28</v>
+      </c>
+      <c r="S3" s="2">
+        <v>48</v>
+      </c>
+      <c r="T3" s="2">
+        <v>85</v>
+      </c>
+      <c r="U3" s="2">
+        <v>58</v>
+      </c>
+      <c r="V3" s="2">
+        <v>-3</v>
+      </c>
+      <c r="W3" s="2">
+        <v>48</v>
+      </c>
+      <c r="X3" s="2">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2">
+        <v>67</v>
+      </c>
+      <c r="D4" s="2">
+        <v>46</v>
+      </c>
+      <c r="E4" s="2">
+        <v>46</v>
+      </c>
+      <c r="F4" s="2">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2">
+        <v>60</v>
+      </c>
+      <c r="H4" s="2">
+        <v>71</v>
+      </c>
+      <c r="I4" s="2">
+        <v>23</v>
+      </c>
+      <c r="J4" s="2">
+        <v>28</v>
+      </c>
+      <c r="K4" s="2">
+        <v>51</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>41</v>
+      </c>
+      <c r="N4" s="2">
+        <v>55</v>
+      </c>
+      <c r="O4" s="2">
+        <v>39</v>
+      </c>
+      <c r="P4" s="2">
+        <v>47</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>56</v>
+      </c>
+      <c r="R4" s="2">
+        <v>85</v>
+      </c>
+      <c r="S4" s="2">
+        <v>51</v>
+      </c>
+      <c r="T4" s="2">
+        <v>92</v>
+      </c>
+      <c r="U4" s="2">
+        <v>36</v>
+      </c>
+      <c r="V4" s="2">
+        <v>88</v>
+      </c>
+      <c r="W4" s="2">
+        <v>85</v>
+      </c>
+      <c r="X4" s="2">
+        <v>67</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2">
+        <v>67</v>
+      </c>
+      <c r="C5" s="2">
+        <v>69</v>
+      </c>
+      <c r="D5" s="2">
+        <v>56</v>
+      </c>
+      <c r="E5" s="2">
+        <v>60</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46</v>
+      </c>
+      <c r="G5" s="2">
+        <v>51</v>
+      </c>
+      <c r="H5" s="2">
+        <v>6</v>
+      </c>
+      <c r="I5" s="2">
+        <v>9</v>
+      </c>
+      <c r="J5" s="2">
+        <v>24</v>
+      </c>
+      <c r="K5" s="2">
+        <v>87</v>
+      </c>
+      <c r="L5" s="2">
+        <v>19</v>
+      </c>
+      <c r="M5" s="2">
+        <v>7</v>
+      </c>
+      <c r="N5" s="2">
+        <v>50</v>
+      </c>
+      <c r="O5" s="2">
+        <v>54</v>
+      </c>
+      <c r="P5" s="2">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>37</v>
+      </c>
+      <c r="R5" s="2">
+        <v>67</v>
+      </c>
+      <c r="S5" s="2">
+        <v>67</v>
+      </c>
+      <c r="T5" s="2">
+        <v>61</v>
+      </c>
+      <c r="U5" s="2">
+        <v>58</v>
+      </c>
+      <c r="V5" s="2">
+        <v>91</v>
+      </c>
+      <c r="W5" s="2">
+        <v>77</v>
+      </c>
+      <c r="X5" s="2">
+        <v>57</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="2">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2">
+        <v>27</v>
+      </c>
+      <c r="G6" s="2">
+        <v>31</v>
+      </c>
+      <c r="H6" s="2">
+        <v>42</v>
+      </c>
+      <c r="I6" s="2">
+        <v>16</v>
+      </c>
+      <c r="J6" s="2">
+        <v>-8</v>
+      </c>
+      <c r="K6" s="2">
+        <v>4</v>
+      </c>
+      <c r="L6" s="2">
+        <v>-36</v>
+      </c>
+      <c r="M6" s="2">
+        <v>16</v>
+      </c>
+      <c r="N6" s="2">
+        <v>27</v>
+      </c>
+      <c r="O6" s="2">
+        <v>24</v>
+      </c>
+      <c r="P6" s="2">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>23</v>
+      </c>
+      <c r="R6" s="2">
+        <v>46</v>
+      </c>
+      <c r="S6" s="2">
+        <v>5</v>
+      </c>
+      <c r="T6" s="2">
+        <v>27</v>
+      </c>
+      <c r="U6" s="2">
+        <v>29</v>
+      </c>
+      <c r="V6" s="2">
+        <v>42</v>
+      </c>
+      <c r="W6" s="2">
+        <v>9</v>
+      </c>
+      <c r="X6" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2">
+        <v>47</v>
+      </c>
+      <c r="D7" s="2">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2">
+        <v>40</v>
+      </c>
+      <c r="F7" s="2">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2">
+        <v>-13</v>
+      </c>
+      <c r="I7" s="2">
+        <v>25</v>
+      </c>
+      <c r="J7" s="2">
+        <v>6</v>
+      </c>
+      <c r="K7" s="2">
+        <v>22</v>
+      </c>
+      <c r="L7" s="2">
+        <v>37</v>
+      </c>
+      <c r="M7" s="2">
+        <v>25</v>
+      </c>
+      <c r="N7" s="2">
+        <v>15</v>
+      </c>
+      <c r="O7" s="2">
+        <v>-9</v>
+      </c>
+      <c r="P7" s="2">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>7</v>
+      </c>
+      <c r="R7" s="2">
+        <v>13</v>
+      </c>
+      <c r="S7" s="2">
+        <v>15</v>
+      </c>
+      <c r="T7" s="2">
+        <v>13</v>
+      </c>
+      <c r="U7" s="2">
+        <v>45</v>
+      </c>
+      <c r="V7" s="2">
+        <v>54</v>
+      </c>
+      <c r="W7" s="2">
+        <v>24</v>
+      </c>
+      <c r="X7" s="2">
+        <v>-5</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-10</v>
+      </c>
+      <c r="C8" s="2">
+        <v>42</v>
+      </c>
+      <c r="D8" s="2">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2">
+        <v>22</v>
+      </c>
+      <c r="F8" s="2">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-6</v>
+      </c>
+      <c r="H8" s="2">
+        <v>24</v>
+      </c>
+      <c r="I8" s="2">
+        <v>31</v>
+      </c>
+      <c r="J8" s="2">
+        <v>35</v>
+      </c>
+      <c r="K8" s="2">
+        <v>-4</v>
+      </c>
+      <c r="L8" s="2">
+        <v>34</v>
+      </c>
+      <c r="M8" s="2">
+        <v>-35</v>
+      </c>
+      <c r="N8" s="2">
+        <v>17</v>
+      </c>
+      <c r="O8" s="2">
+        <v>29</v>
+      </c>
+      <c r="P8" s="2">
+        <v>38</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>27</v>
+      </c>
+      <c r="R8" s="2">
+        <v>41</v>
+      </c>
+      <c r="S8" s="2">
+        <v>16</v>
+      </c>
+      <c r="T8" s="2">
+        <v>34</v>
+      </c>
+      <c r="U8" s="2">
+        <v>-10</v>
+      </c>
+      <c r="V8" s="2">
+        <v>47</v>
+      </c>
+      <c r="W8" s="2">
+        <v>30</v>
+      </c>
+      <c r="X8" s="2">
+        <v>22</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>-22</v>
+      </c>
+      <c r="F9" s="2">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2">
+        <v>9</v>
+      </c>
+      <c r="H9" s="2">
+        <v>13</v>
+      </c>
+      <c r="I9" s="2">
+        <v>7</v>
+      </c>
+      <c r="J9" s="2">
+        <v>52</v>
+      </c>
+      <c r="K9" s="2">
+        <v>26</v>
+      </c>
+      <c r="L9" s="2">
+        <v>45</v>
+      </c>
+      <c r="M9" s="2">
+        <v>14</v>
+      </c>
+      <c r="N9" s="2">
+        <v>24</v>
+      </c>
+      <c r="O9" s="2">
+        <v>35</v>
+      </c>
+      <c r="P9" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>-2</v>
+      </c>
+      <c r="R9" s="2">
+        <v>17</v>
+      </c>
+      <c r="S9" s="2">
+        <v>-4</v>
+      </c>
+      <c r="T9" s="2">
+        <v>25</v>
+      </c>
+      <c r="U9" s="2">
+        <v>2</v>
+      </c>
+      <c r="V9" s="2">
+        <v>-9</v>
+      </c>
+      <c r="W9" s="2">
+        <v>-8</v>
+      </c>
+      <c r="X9" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2">
+        <v>18</v>
+      </c>
+      <c r="F10" s="2">
+        <v>11</v>
+      </c>
+      <c r="G10" s="2">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2">
+        <v>14</v>
+      </c>
+      <c r="I10" s="2">
+        <v>-4</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>31</v>
+      </c>
+      <c r="L10" s="2">
+        <v>24</v>
+      </c>
+      <c r="M10" s="2">
+        <v>33</v>
+      </c>
+      <c r="N10" s="2">
+        <v>20</v>
+      </c>
+      <c r="O10" s="2">
+        <v>45</v>
+      </c>
+      <c r="P10" s="2">
+        <v>41</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>-11</v>
+      </c>
+      <c r="R10" s="2">
+        <v>-2</v>
+      </c>
+      <c r="S10" s="2">
+        <v>37</v>
+      </c>
+      <c r="T10" s="2">
+        <v>-12</v>
+      </c>
+      <c r="U10" s="2">
+        <v>2</v>
+      </c>
+      <c r="V10" s="2">
+        <v>9</v>
+      </c>
+      <c r="W10" s="2">
+        <v>-8</v>
+      </c>
+      <c r="X10" s="2">
+        <v>21</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2">
+        <v>-14</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>9</v>
+      </c>
+      <c r="E11" s="2">
+        <v>22</v>
+      </c>
+      <c r="F11" s="2">
+        <v>-6</v>
+      </c>
+      <c r="G11" s="2">
+        <v>10</v>
+      </c>
+      <c r="H11" s="2">
+        <v>10</v>
+      </c>
+      <c r="I11" s="2">
+        <v>-11</v>
+      </c>
+      <c r="J11" s="2">
+        <v>31</v>
+      </c>
+      <c r="K11" s="2">
+        <v>11</v>
+      </c>
+      <c r="L11" s="2">
+        <v>17</v>
+      </c>
+      <c r="M11" s="2">
+        <v>5</v>
+      </c>
+      <c r="N11" s="2">
+        <v>-13</v>
+      </c>
+      <c r="O11" s="2">
+        <v>2</v>
+      </c>
+      <c r="P11" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>6</v>
+      </c>
+      <c r="R11" s="2">
+        <v>7</v>
+      </c>
+      <c r="S11" s="2">
+        <v>6</v>
+      </c>
+      <c r="T11" s="2">
+        <v>18</v>
+      </c>
+      <c r="U11" s="2">
+        <v>14</v>
+      </c>
+      <c r="V11" s="2">
+        <v>12</v>
+      </c>
+      <c r="W11" s="2">
+        <v>3</v>
+      </c>
+      <c r="X11" s="2">
+        <v>14</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED373387-C4B1-4C53-B689-3A35B6C15A04}">
+  <dimension ref="A1:Z24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="X31" sqref="X30:X31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A1" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -3122,8 +3155,11 @@
       <c r="Y1" s="3">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:25">
+      <c r="Z1" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -3199,8 +3235,11 @@
       <c r="Y2" s="2">
         <v>30.4</v>
       </c>
-    </row>
-    <row r="3" spans="1:25">
+      <c r="Z2" s="2">
+        <v>30.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -3276,8 +3315,11 @@
       <c r="Y3" s="2">
         <v>29.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:25">
+      <c r="Z3" s="2">
+        <v>30.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3353,8 +3395,11 @@
       <c r="Y4" s="2">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:25">
+      <c r="Z4" s="2">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -3430,8 +3475,11 @@
       <c r="Y5" s="2">
         <v>23.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:25">
+      <c r="Z5" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -3507,8 +3555,11 @@
       <c r="Y6" s="2">
         <v>22.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:25">
+      <c r="Z6" s="2">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -3584,8 +3635,11 @@
       <c r="Y7" s="2">
         <v>23.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:25">
+      <c r="Z7" s="2">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -3619,8 +3673,9 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
-    </row>
-    <row r="9" spans="1:25">
+      <c r="Z8" s="2"/>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
@@ -3696,8 +3751,11 @@
       <c r="Y9" s="2">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:25">
+      <c r="Z9" s="2">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -3769,8 +3827,11 @@
       <c r="Y10" s="2">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:25">
+      <c r="Z10" s="2">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -3846,8 +3907,11 @@
       <c r="Y11" s="2">
         <v>13.2</v>
       </c>
-    </row>
-    <row r="12" spans="1:25">
+      <c r="Z11" s="2">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -3881,8 +3945,9 @@
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
-    </row>
-    <row r="13" spans="1:25">
+      <c r="Z12" s="2"/>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -3958,8 +4023,11 @@
       <c r="Y13" s="2">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="14" spans="1:25">
+      <c r="Z13" s="2">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -4035,8 +4103,11 @@
       <c r="Y14" s="2">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:25">
+      <c r="Z14" s="2">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -4112,8 +4183,11 @@
       <c r="Y15" s="2">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="16" spans="1:25">
+      <c r="Z15" s="2">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -4189,8 +4263,11 @@
       <c r="Y16" s="2">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="17" spans="1:25">
+      <c r="Z16" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -4266,8 +4343,11 @@
       <c r="Y17" s="2">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:25">
+      <c r="Z17" s="2">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
@@ -4343,8 +4423,11 @@
       <c r="Y18" s="2">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="19" spans="1:25">
+      <c r="Z18" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
       <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
@@ -4420,8 +4503,11 @@
       <c r="Y19" s="2">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:25">
+      <c r="Z19" s="2">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
       <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
@@ -4463,8 +4549,9 @@
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
-    </row>
-    <row r="21" spans="1:25">
+      <c r="Z20" s="2"/>
+    </row>
+    <row r="21" spans="1:26">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
@@ -4540,8 +4627,11 @@
       <c r="Y21" s="2">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="22" spans="1:25">
+      <c r="Z21" s="2">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -4613,8 +4703,11 @@
       <c r="Y22" s="2">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:25">
+      <c r="Z22" s="2">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26">
       <c r="A23" s="2" t="s">
         <v>39</v>
       </c>
@@ -4690,8 +4783,11 @@
       <c r="Y23" s="2">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="24" spans="1:25">
+      <c r="Z23" s="2">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -4755,6 +4851,9 @@
       <c r="Y24" s="2">
         <v>4.5</v>
       </c>
+      <c r="Z24" s="2">
+        <v>4.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4763,13 +4862,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C15A70-BFDE-46F9-9F77-0BE1119DCB97}">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W25" sqref="W25"/>
+      <selection pane="bottomRight" activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4777,7 +4876,7 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="4" customFormat="1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:25" s="4" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>41</v>
       </c>
@@ -4850,8 +4949,11 @@
       <c r="X1" s="3">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:24">
+      <c r="Y1" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -4924,8 +5026,11 @@
       <c r="X2" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="Y2" s="2">
+        <v>36.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -4998,8 +5103,11 @@
       <c r="X3" s="2">
         <v>31.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="Y3" s="2">
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -5072,8 +5180,11 @@
       <c r="X4" s="2">
         <v>30.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="Y4" s="2">
+        <v>31.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -5146,8 +5257,11 @@
       <c r="X5" s="2">
         <v>28.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="Y5" s="2">
+        <v>28.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -5220,8 +5334,11 @@
       <c r="X6" s="2">
         <v>19.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="Y6" s="2">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
@@ -5294,8 +5411,11 @@
       <c r="X7" s="2">
         <v>15.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="Y7" s="2">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -5368,8 +5488,11 @@
       <c r="X8" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="Y8" s="2">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -5442,8 +5565,11 @@
       <c r="X9" s="2">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:24">
+      <c r="Y9" s="2">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -5516,8 +5642,11 @@
       <c r="X10" s="2">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="Y10" s="2">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -5589,6 +5718,9 @@
       </c>
       <c r="X11" s="2">
         <v>9.3000000000000007</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>8.6999999999999993</v>
       </c>
     </row>
   </sheetData>
@@ -14295,13 +14427,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11985E4F-6F4E-4304-AF61-8A6F49D5D125}">
-  <dimension ref="A1:Y24"/>
+  <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y23" sqref="Y23"/>
+      <selection pane="bottomRight" activeCell="X29" sqref="X29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14309,7 +14441,7 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:26" s="4" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>40</v>
       </c>
@@ -14385,8 +14517,11 @@
       <c r="Y1" s="3">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:25">
+      <c r="Z1" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -14460,10 +14595,13 @@
         <v>-10</v>
       </c>
       <c r="Y2" s="2">
+        <v>25</v>
+      </c>
+      <c r="Z2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:26">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -14537,10 +14675,13 @@
         <v>-14</v>
       </c>
       <c r="Y3" s="2">
+        <v>46</v>
+      </c>
+      <c r="Z3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:26">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -14614,10 +14755,13 @@
         <v>56</v>
       </c>
       <c r="Y4" s="2">
+        <v>55</v>
+      </c>
+      <c r="Z4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:26">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -14691,10 +14835,13 @@
         <v>30</v>
       </c>
       <c r="Y5" s="2">
+        <v>22</v>
+      </c>
+      <c r="Z5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:26">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -14768,10 +14915,13 @@
         <v>18</v>
       </c>
       <c r="Y6" s="2">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:26">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -14845,10 +14995,13 @@
         <v>23</v>
       </c>
       <c r="Y7" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:26">
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
@@ -14922,10 +15075,13 @@
         <v>32</v>
       </c>
       <c r="Y8" s="2">
+        <v>23</v>
+      </c>
+      <c r="Z8" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:26">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -14999,10 +15155,13 @@
         <v>-17</v>
       </c>
       <c r="Y9" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z9" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:26">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -15076,10 +15235,13 @@
         <v>10</v>
       </c>
       <c r="Y10" s="2">
+        <v>-17</v>
+      </c>
+      <c r="Z10" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:26">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -15149,10 +15311,13 @@
         <v>9</v>
       </c>
       <c r="Y11" s="2">
+        <v>12</v>
+      </c>
+      <c r="Z11" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:26">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -15226,10 +15391,13 @@
         <v>-20</v>
       </c>
       <c r="Y12" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z12" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:26">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -15303,10 +15471,13 @@
         <v>11</v>
       </c>
       <c r="Y13" s="2">
+        <v>-18</v>
+      </c>
+      <c r="Z13" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:26">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -15380,10 +15551,13 @@
         <v>9</v>
       </c>
       <c r="Y14" s="2">
+        <v>6</v>
+      </c>
+      <c r="Z14" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:26">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
@@ -15457,10 +15631,13 @@
         <v>16</v>
       </c>
       <c r="Y15" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:26">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -15534,10 +15711,13 @@
         <v>-20</v>
       </c>
       <c r="Y16" s="2">
+        <v>14</v>
+      </c>
+      <c r="Z16" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:26">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -15611,10 +15791,13 @@
         <v>16</v>
       </c>
       <c r="Y17" s="2">
+        <v>27</v>
+      </c>
+      <c r="Z17" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:26">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -15648,8 +15831,9 @@
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
-    </row>
-    <row r="19" spans="1:25">
+      <c r="Z18" s="2"/>
+    </row>
+    <row r="19" spans="1:26">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -15683,8 +15867,9 @@
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
-    </row>
-    <row r="20" spans="1:25">
+      <c r="Z19" s="2"/>
+    </row>
+    <row r="20" spans="1:26">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -15754,10 +15939,13 @@
         <v>-1</v>
       </c>
       <c r="Y20" s="2">
+        <v>11</v>
+      </c>
+      <c r="Z20" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:26">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -15831,10 +16019,13 @@
         <v>-2</v>
       </c>
       <c r="Y21" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z21" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:26">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -15896,10 +16087,13 @@
         <v>0</v>
       </c>
       <c r="Y22" s="2">
+        <v>6</v>
+      </c>
+      <c r="Z22" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:26">
       <c r="A23" s="2" t="s">
         <v>4</v>
       </c>
@@ -15973,10 +16167,13 @@
         <v>2</v>
       </c>
       <c r="Y23" s="2">
+        <v>12</v>
+      </c>
+      <c r="Z23" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:26">
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Added '26 line-up, with test prices
</commit_message>
<xml_diff>
--- a/data/f1_fantasy_archive.xlsx
+++ b/data/f1_fantasy_archive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexs\Dropbox\Dev\f1_fantasy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3185CAA-CEBA-478E-886E-6B3A735128D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973D215F-5F94-4D73-B947-70F9C08B7367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="8" activeTab="9" xr2:uid="{5075C4C2-DC0E-48A5-BDF1-482703F248E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="13" xr2:uid="{5075C4C2-DC0E-48A5-BDF1-482703F248E6}"/>
   </bookViews>
   <sheets>
     <sheet name="2023 Drivers Points" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,10 @@
     <sheet name="2025 Constructors Points" sheetId="6" r:id="rId10"/>
     <sheet name="2025 Drivers Price" sheetId="11" r:id="rId11"/>
     <sheet name="2025 Constructors Price" sheetId="12" r:id="rId12"/>
+    <sheet name="2026 Drivers Points" sheetId="13" r:id="rId13"/>
+    <sheet name="2026 Constructors Points" sheetId="14" r:id="rId14"/>
+    <sheet name="2026 Drivers Price" sheetId="15" r:id="rId15"/>
+    <sheet name="2026 Constructors Price" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="44">
   <si>
     <t>VER</t>
   </si>
@@ -162,6 +166,12 @@
   </si>
   <si>
     <t>Team</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>LIN</t>
   </si>
 </sst>
 </file>
@@ -2199,11 +2209,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2707B16-05A3-42D1-BE37-AF149E8BEDBE}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R22" sqref="R22"/>
+      <selection activeCell="R25" sqref="R25"/>
+      <selection pane="topRight" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomLeft" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomRight" activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3069,9 +3080,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X31" sqref="X30:X31"/>
+      <selection activeCell="R25" sqref="R25"/>
+      <selection pane="topRight" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomLeft" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomRight" activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4866,9 +4878,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R25" sqref="R25"/>
+      <selection activeCell="R25" sqref="R25"/>
+      <selection pane="topRight" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomLeft" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomRight" activeCell="Y2" sqref="Y2:Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5720,6 +5733,807 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="Y11" s="2">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C694E7B-FEFC-4A8B-96D9-423EDFAEB881}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="R25" sqref="R25"/>
+      <selection pane="topRight" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomLeft" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6D707-49FB-4CAF-A537-BEE4CA75B4FC}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="R25" sqref="R25"/>
+      <selection pane="topRight" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomLeft" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomRight" activeCell="K30" sqref="K30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4905D1-CA76-4C74-B555-02BE6E027F80}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="R25" sqref="R25"/>
+      <selection pane="topRight" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomLeft" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2">
+        <v>30.3</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="2">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>30.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>21.9</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5.9</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="2">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="2">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16AA477-ED3B-48C2-94B3-EDD2D119BA86}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="R25" sqref="R25"/>
+      <selection pane="topRight" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomLeft" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomRight" activeCell="O35" sqref="O35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2">
+        <v>36.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2">
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2">
+        <v>31.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2">
+        <v>28.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="2">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="2">
         <v>8.6999999999999993</v>
       </c>
     </row>
@@ -14431,9 +15245,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z24" sqref="Z24"/>
+      <selection activeCell="R25" sqref="R25"/>
+      <selection pane="topRight" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomLeft" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomRight" activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updated '26 line-up with test prices
</commit_message>
<xml_diff>
--- a/data/f1_fantasy_archive.xlsx
+++ b/data/f1_fantasy_archive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexs\Dropbox\Dev\f1_fantasy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973D215F-5F94-4D73-B947-70F9C08B7367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98229F0-2B07-4F07-A68F-AC4F3D4F854E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="13" xr2:uid="{5075C4C2-DC0E-48A5-BDF1-482703F248E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="14" xr2:uid="{5075C4C2-DC0E-48A5-BDF1-482703F248E6}"/>
   </bookViews>
   <sheets>
     <sheet name="2023 Drivers Points" sheetId="1" r:id="rId1"/>
@@ -5750,7 +5750,7 @@
       <selection activeCell="R25" sqref="R25"/>
       <selection pane="topRight" activeCell="R25" sqref="R25"/>
       <selection pane="bottomLeft" activeCell="R25" sqref="R25"/>
-      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5793,10 +5793,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -5804,10 +5804,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -5815,10 +5815,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>0</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -5826,10 +5826,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
@@ -5837,10 +5837,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
@@ -5848,10 +5848,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
@@ -5859,10 +5859,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
@@ -5870,10 +5870,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="C11" s="2">
         <v>0</v>
@@ -5881,10 +5881,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -5892,10 +5892,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="C13" s="2">
         <v>0</v>
@@ -5903,10 +5903,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="C14" s="2">
         <v>0</v>
@@ -5914,10 +5914,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C15" s="2">
         <v>0</v>
@@ -5925,10 +5925,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C16" s="2">
         <v>0</v>
@@ -5936,10 +5936,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
@@ -5947,10 +5947,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C18" s="2">
         <v>0</v>
@@ -5958,10 +5958,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="C19" s="2">
         <v>0</v>
@@ -5969,10 +5969,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="C20" s="2">
         <v>0</v>
@@ -5980,10 +5980,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C21" s="2">
         <v>0</v>
@@ -5991,10 +5991,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C22" s="2">
         <v>0</v>
@@ -6002,10 +6002,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C23" s="2">
         <v>0</v>
@@ -6025,7 +6025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6D707-49FB-4CAF-A537-BEE4CA75B4FC}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="R25" sqref="R25"/>
       <selection pane="topRight" activeCell="R25" sqref="R25"/>
@@ -6143,12 +6143,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4905D1-CA76-4C74-B555-02BE6E027F80}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="R25" sqref="R25"/>
       <selection pane="topRight" activeCell="R25" sqref="R25"/>
       <selection pane="bottomLeft" activeCell="R25" sqref="R25"/>
-      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6192,10 +6192,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>23.7</v>
@@ -6203,10 +6203,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="C5" s="2">
         <v>18.100000000000001</v>
@@ -6214,10 +6214,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>0</v>
       </c>
       <c r="C6" s="2">
         <v>30.1</v>
@@ -6225,10 +6225,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C7" s="2">
         <v>6.9</v>
@@ -6236,10 +6236,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="C8" s="2">
         <v>21.9</v>
@@ -6248,10 +6248,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C9" s="2">
         <v>23</v>
@@ -6259,10 +6259,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="C10" s="2">
         <v>12.6</v>
@@ -6271,10 +6271,10 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="C11" s="2">
         <v>7.7</v>
@@ -6282,10 +6282,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="C12" s="2">
         <v>5.9</v>
@@ -6294,10 +6294,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="C13" s="2">
         <v>4.5</v>
@@ -6305,10 +6305,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="C14" s="2">
         <v>4.7</v>
@@ -6316,10 +6316,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C15" s="2">
         <v>6.7</v>
@@ -6327,10 +6327,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C16" s="2">
         <v>7.9</v>
@@ -6338,10 +6338,10 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C17" s="2">
         <v>9.3000000000000007</v>
@@ -6349,10 +6349,10 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C18" s="2">
         <v>5</v>
@@ -6360,10 +6360,10 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="C19" s="2">
         <v>5.5</v>
@@ -6371,10 +6371,10 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="C20" s="2">
         <v>6.5</v>
@@ -6383,10 +6383,10 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C21" s="2">
         <v>4.5</v>
@@ -6394,10 +6394,10 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C22" s="2">
         <v>4.5</v>
@@ -6405,10 +6405,10 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C23" s="2">
         <v>4.5</v>

</xml_diff>